<commit_message>
ant and greedyKNN available
</commit_message>
<xml_diff>
--- a/TSP/output.xlsx
+++ b/TSP/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B68CC-1117-4F9C-91AA-42647C5EFDB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA12879-1A73-41AA-A540-4E9CE43AB31D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="briefOutput_1" localSheetId="0">Sheet1!$A$1:$BF$9</definedName>
+    <definedName name="briefOutput_1" localSheetId="0">Sheet1!$A$1:$BF$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{B4183C22-7F1C-4622-BF7D-79481EA14B11}" name="briefOutput" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" xr16:uid="{17DF2899-9B80-469F-8091-A3CD22A51120}" name="briefOutput" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="936" sourceFile="C:\Users\66919\TSP-Course-Design\TSP\briefOutput.txt" tab="0" space="1" consecutive="1">
       <textFields count="58">
         <textField/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="189">
   <si>
     <t>berlin52.tsp</t>
   </si>
@@ -211,265 +211,454 @@
     <t>optimal</t>
   </si>
   <si>
-    <t>0.192ms</t>
-  </si>
-  <si>
-    <t>1.5521ms</t>
-  </si>
-  <si>
-    <t>1.471ms</t>
-  </si>
-  <si>
-    <t>1.4567ms</t>
-  </si>
-  <si>
-    <t>3.5124ms</t>
-  </si>
-  <si>
-    <t>0.8298ms</t>
-  </si>
-  <si>
-    <t>0.662ms</t>
-  </si>
-  <si>
-    <t>1.4137ms</t>
-  </si>
-  <si>
-    <t>3.3611ms</t>
-  </si>
-  <si>
-    <t>0.6176ms</t>
-  </si>
-  <si>
-    <t>1.3726ms</t>
-  </si>
-  <si>
-    <t>2.6139ms</t>
-  </si>
-  <si>
-    <t>0.6784ms</t>
-  </si>
-  <si>
-    <t>0.6478ms</t>
-  </si>
-  <si>
-    <t>0.7481ms</t>
-  </si>
-  <si>
-    <t>0.6796ms</t>
-  </si>
-  <si>
-    <t>0.3727ms</t>
-  </si>
-  <si>
-    <t>0.695ms</t>
-  </si>
-  <si>
-    <t>1.0359ms</t>
-  </si>
-  <si>
-    <t>1.2782ms</t>
-  </si>
-  <si>
-    <t>1.2692ms</t>
-  </si>
-  <si>
-    <t>1.5411ms</t>
-  </si>
-  <si>
-    <t>0.8036ms</t>
-  </si>
-  <si>
-    <t>2.2416ms</t>
-  </si>
-  <si>
-    <t>0.7292ms</t>
-  </si>
-  <si>
-    <t>0.3171ms</t>
-  </si>
-  <si>
-    <t>3.5764ms</t>
-  </si>
-  <si>
-    <t>3.1369ms</t>
-  </si>
-  <si>
-    <t>1.5082ms</t>
-  </si>
-  <si>
-    <t>0.242ms</t>
-  </si>
-  <si>
-    <t>1.0921ms</t>
-  </si>
-  <si>
-    <t>0.9919ms</t>
-  </si>
-  <si>
-    <t>1.502ms</t>
-  </si>
-  <si>
-    <t>2.4036ms</t>
-  </si>
-  <si>
-    <t>0.7504ms</t>
-  </si>
-  <si>
-    <t>0.6756ms</t>
-  </si>
-  <si>
-    <t>1.7135ms</t>
-  </si>
-  <si>
-    <t>2.7332ms</t>
-  </si>
-  <si>
-    <t>0.7945ms</t>
-  </si>
-  <si>
-    <t>1.4519ms</t>
-  </si>
-  <si>
-    <t>2.4089ms</t>
-  </si>
-  <si>
-    <t>0.9879ms</t>
-  </si>
-  <si>
-    <t>0.834ms</t>
-  </si>
-  <si>
-    <t>1.1871ms</t>
-  </si>
-  <si>
-    <t>1.2172ms</t>
-  </si>
-  <si>
-    <t>0.6807ms</t>
-  </si>
-  <si>
-    <t>0.947ms</t>
-  </si>
-  <si>
-    <t>1.1504ms</t>
-  </si>
-  <si>
-    <t>1.8133ms</t>
-  </si>
-  <si>
-    <t>1.3844ms</t>
-  </si>
-  <si>
-    <t>1.9515ms</t>
-  </si>
-  <si>
-    <t>0.5992ms</t>
-  </si>
-  <si>
-    <t>2.4067ms</t>
-  </si>
-  <si>
-    <t>0.6534ms</t>
-  </si>
-  <si>
-    <t>0.3324ms</t>
-  </si>
-  <si>
-    <t>5.4767ms</t>
-  </si>
-  <si>
-    <t>3.3878ms</t>
-  </si>
-  <si>
-    <t>1.2617ms</t>
-  </si>
-  <si>
-    <t>190.393ms</t>
-  </si>
-  <si>
-    <t>470.19ms</t>
-  </si>
-  <si>
-    <t>427.21ms</t>
-  </si>
-  <si>
-    <t>468.051ms</t>
-  </si>
-  <si>
-    <t>612.406ms</t>
-  </si>
-  <si>
-    <t>371.067ms</t>
-  </si>
-  <si>
-    <t>364.776ms</t>
-  </si>
-  <si>
-    <t>534.863ms</t>
-  </si>
-  <si>
-    <t>709.079ms</t>
-  </si>
-  <si>
-    <t>357.048ms</t>
-  </si>
-  <si>
-    <t>534.476ms</t>
-  </si>
-  <si>
-    <t>704.775ms</t>
-  </si>
-  <si>
-    <t>372.995ms</t>
-  </si>
-  <si>
-    <t>361.424ms</t>
-  </si>
-  <si>
-    <t>366.267ms</t>
-  </si>
-  <si>
-    <t>377.352ms</t>
-  </si>
-  <si>
-    <t>278.905ms</t>
-  </si>
-  <si>
-    <t>385.694ms</t>
-  </si>
-  <si>
-    <t>441.777ms</t>
-  </si>
-  <si>
-    <t>482.106ms</t>
-  </si>
-  <si>
-    <t>513.166ms</t>
-  </si>
-  <si>
-    <t>538.466ms</t>
-  </si>
-  <si>
-    <t>356.984ms</t>
-  </si>
-  <si>
-    <t>686.66ms</t>
-  </si>
-  <si>
-    <t>325.328ms</t>
-  </si>
-  <si>
-    <t>257.751ms</t>
-  </si>
-  <si>
-    <t>790.407ms</t>
-  </si>
-  <si>
-    <t>739.477ms</t>
-  </si>
-  <si>
-    <t>504.992ms</t>
+    <t>Algo5:</t>
+  </si>
+  <si>
+    <t>Ant</t>
+  </si>
+  <si>
+    <t>Crowd</t>
+  </si>
+  <si>
+    <t>5260.4ms</t>
+  </si>
+  <si>
+    <t>5347.66ms</t>
+  </si>
+  <si>
+    <t>4767.14ms</t>
+  </si>
+  <si>
+    <t>4733.98ms</t>
+  </si>
+  <si>
+    <t>3949.2ms</t>
+  </si>
+  <si>
+    <t>4313.67ms</t>
+  </si>
+  <si>
+    <t>4310.25ms</t>
+  </si>
+  <si>
+    <t>4338.98ms</t>
+  </si>
+  <si>
+    <t>4259.5ms</t>
+  </si>
+  <si>
+    <t>4284.98ms</t>
+  </si>
+  <si>
+    <t>4370.26ms</t>
+  </si>
+  <si>
+    <t>4249.29ms</t>
+  </si>
+  <si>
+    <t>4180.57ms</t>
+  </si>
+  <si>
+    <t>4236.35ms</t>
+  </si>
+  <si>
+    <t>4236.66ms</t>
+  </si>
+  <si>
+    <t>4241.68ms</t>
+  </si>
+  <si>
+    <t>4284.78ms</t>
+  </si>
+  <si>
+    <t>4422.44ms</t>
+  </si>
+  <si>
+    <t>4293.66ms</t>
+  </si>
+  <si>
+    <t>6219.8ms</t>
+  </si>
+  <si>
+    <t>4295.97ms</t>
+  </si>
+  <si>
+    <t>4348.34ms</t>
+  </si>
+  <si>
+    <t>4279.7ms</t>
+  </si>
+  <si>
+    <t>4259.25ms</t>
+  </si>
+  <si>
+    <t>4121.73ms</t>
+  </si>
+  <si>
+    <t>4271.65ms</t>
+  </si>
+  <si>
+    <t>4252.07ms</t>
+  </si>
+  <si>
+    <t>3815.7ms</t>
+  </si>
+  <si>
+    <t>4480.63ms</t>
+  </si>
+  <si>
+    <t>0.1803ms</t>
+  </si>
+  <si>
+    <t>0.9803ms</t>
+  </si>
+  <si>
+    <t>1.1154ms</t>
+  </si>
+  <si>
+    <t>1.2861ms</t>
+  </si>
+  <si>
+    <t>2.1791ms</t>
+  </si>
+  <si>
+    <t>0.6375ms</t>
+  </si>
+  <si>
+    <t>0.704ms</t>
+  </si>
+  <si>
+    <t>1.4015ms</t>
+  </si>
+  <si>
+    <t>4.9262ms</t>
+  </si>
+  <si>
+    <t>0.6377ms</t>
+  </si>
+  <si>
+    <t>1.789ms</t>
+  </si>
+  <si>
+    <t>2.3914ms</t>
+  </si>
+  <si>
+    <t>0.6278ms</t>
+  </si>
+  <si>
+    <t>0.7888ms</t>
+  </si>
+  <si>
+    <t>0.7142ms</t>
+  </si>
+  <si>
+    <t>0.7259ms</t>
+  </si>
+  <si>
+    <t>0.3744ms</t>
+  </si>
+  <si>
+    <t>0.7234ms</t>
+  </si>
+  <si>
+    <t>1.4656ms</t>
+  </si>
+  <si>
+    <t>1.1267ms</t>
+  </si>
+  <si>
+    <t>1.2605ms</t>
+  </si>
+  <si>
+    <t>1.6016ms</t>
+  </si>
+  <si>
+    <t>0.6103ms</t>
+  </si>
+  <si>
+    <t>3.2973ms</t>
+  </si>
+  <si>
+    <t>0.7731ms</t>
+  </si>
+  <si>
+    <t>0.3182ms</t>
+  </si>
+  <si>
+    <t>2.9669ms</t>
+  </si>
+  <si>
+    <t>2.9109ms</t>
+  </si>
+  <si>
+    <t>1.4607ms</t>
+  </si>
+  <si>
+    <t>0.1581ms</t>
+  </si>
+  <si>
+    <t>0.931ms</t>
+  </si>
+  <si>
+    <t>1.2971ms</t>
+  </si>
+  <si>
+    <t>1.27ms</t>
+  </si>
+  <si>
+    <t>2.0017ms</t>
+  </si>
+  <si>
+    <t>0.6252ms</t>
+  </si>
+  <si>
+    <t>0.6266ms</t>
+  </si>
+  <si>
+    <t>1.41ms</t>
+  </si>
+  <si>
+    <t>3.3162ms</t>
+  </si>
+  <si>
+    <t>0.6578ms</t>
+  </si>
+  <si>
+    <t>1.4763ms</t>
+  </si>
+  <si>
+    <t>2.9671ms</t>
+  </si>
+  <si>
+    <t>0.6566ms</t>
+  </si>
+  <si>
+    <t>0.7343ms</t>
+  </si>
+  <si>
+    <t>1.0932ms</t>
+  </si>
+  <si>
+    <t>0.7136ms</t>
+  </si>
+  <si>
+    <t>0.4837ms</t>
+  </si>
+  <si>
+    <t>0.758ms</t>
+  </si>
+  <si>
+    <t>1.2284ms</t>
+  </si>
+  <si>
+    <t>1.6024ms</t>
+  </si>
+  <si>
+    <t>1.3456ms</t>
+  </si>
+  <si>
+    <t>2.1371ms</t>
+  </si>
+  <si>
+    <t>0.7166ms</t>
+  </si>
+  <si>
+    <t>2.2502ms</t>
+  </si>
+  <si>
+    <t>0.6579ms</t>
+  </si>
+  <si>
+    <t>0.3425ms</t>
+  </si>
+  <si>
+    <t>2.9906ms</t>
+  </si>
+  <si>
+    <t>2.6189ms</t>
+  </si>
+  <si>
+    <t>1.8839ms</t>
+  </si>
+  <si>
+    <t>126.888ms</t>
+  </si>
+  <si>
+    <t>485.986ms</t>
+  </si>
+  <si>
+    <t>1977.38ms</t>
+  </si>
+  <si>
+    <t>2886.31ms</t>
+  </si>
+  <si>
+    <t>6740.94ms</t>
+  </si>
+  <si>
+    <t>359.45ms</t>
+  </si>
+  <si>
+    <t>364.947ms</t>
+  </si>
+  <si>
+    <t>566.964ms</t>
+  </si>
+  <si>
+    <t>713.717ms</t>
+  </si>
+  <si>
+    <t>361.662ms</t>
+  </si>
+  <si>
+    <t>532.448ms</t>
+  </si>
+  <si>
+    <t>768.943ms</t>
+  </si>
+  <si>
+    <t>376.425ms</t>
+  </si>
+  <si>
+    <t>375.237ms</t>
+  </si>
+  <si>
+    <t>363.154ms</t>
+  </si>
+  <si>
+    <t>394.485ms</t>
+  </si>
+  <si>
+    <t>278.569ms</t>
+  </si>
+  <si>
+    <t>389.051ms</t>
+  </si>
+  <si>
+    <t>445.433ms</t>
+  </si>
+  <si>
+    <t>490.126ms</t>
+  </si>
+  <si>
+    <t>521.68ms</t>
+  </si>
+  <si>
+    <t>543.499ms</t>
+  </si>
+  <si>
+    <t>356.403ms</t>
+  </si>
+  <si>
+    <t>688.488ms</t>
+  </si>
+  <si>
+    <t>881.531ms</t>
+  </si>
+  <si>
+    <t>289.399ms</t>
+  </si>
+  <si>
+    <t>800.752ms</t>
+  </si>
+  <si>
+    <t>11739.9ms</t>
+  </si>
+  <si>
+    <t>3141.41ms</t>
+  </si>
+  <si>
+    <t>Algo4:</t>
+  </si>
+  <si>
+    <t>greedyKNN</t>
+  </si>
+  <si>
+    <t>0.1301ms</t>
+  </si>
+  <si>
+    <t>1.6658ms</t>
+  </si>
+  <si>
+    <t>1.7893ms</t>
+  </si>
+  <si>
+    <t>2.6644ms</t>
+  </si>
+  <si>
+    <t>6.0405ms</t>
+  </si>
+  <si>
+    <t>0.8405ms</t>
+  </si>
+  <si>
+    <t>0.8275ms</t>
+  </si>
+  <si>
+    <t>4.1504ms</t>
+  </si>
+  <si>
+    <t>6.1197ms</t>
+  </si>
+  <si>
+    <t>0.871ms</t>
+  </si>
+  <si>
+    <t>2.7986ms</t>
+  </si>
+  <si>
+    <t>7.0579ms</t>
+  </si>
+  <si>
+    <t>1.0396ms</t>
+  </si>
+  <si>
+    <t>0.9319ms</t>
+  </si>
+  <si>
+    <t>0.825ms</t>
+  </si>
+  <si>
+    <t>0.9345ms</t>
+  </si>
+  <si>
+    <t>0.4019ms</t>
+  </si>
+  <si>
+    <t>1.2669ms</t>
+  </si>
+  <si>
+    <t>1.6327ms</t>
+  </si>
+  <si>
+    <t>1.9897ms</t>
+  </si>
+  <si>
+    <t>2.6261ms</t>
+  </si>
+  <si>
+    <t>2.8253ms</t>
+  </si>
+  <si>
+    <t>0.7843ms</t>
+  </si>
+  <si>
+    <t>5.9286ms</t>
+  </si>
+  <si>
+    <t>0.847ms</t>
+  </si>
+  <si>
+    <t>0.3195ms</t>
+  </si>
+  <si>
+    <t>9.6308ms</t>
+  </si>
+  <si>
+    <t>8.9106ms</t>
+  </si>
+  <si>
+    <t>3.2304ms</t>
   </si>
 </sst>
 </file>
@@ -532,7 +721,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="briefOutput_1" connectionId="1" xr16:uid="{9409DDCF-318C-4A6D-8BD8-2BD1699B5935}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="briefOutput_1" connectionId="1" xr16:uid="{FEBA5FEE-30F3-4377-9FD9-21063A689EC8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -798,20 +987,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF9"/>
+  <dimension ref="A1:BF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -838,7 +1026,7 @@
     <col min="30" max="30" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -853,7 +1041,7 @@
     <col min="45" max="45" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="8.5546875" bestFit="1" customWidth="1"/>
@@ -1044,197 +1232,197 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8612.89</v>
+        <v>8511.58</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C3">
-        <v>137075</v>
+        <v>408478</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E3">
-        <v>6936.37</v>
+        <v>6965.39</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G3">
-        <v>7494.25</v>
+        <v>7534.85</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I3">
-        <v>17364.400000000001</v>
+        <v>17867</v>
       </c>
       <c r="J3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K3">
-        <v>710.47699999999998</v>
+        <v>2142.5300000000002</v>
       </c>
       <c r="L3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M3">
-        <v>25018.799999999999</v>
+        <v>182798</v>
       </c>
       <c r="N3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O3">
-        <v>30444.6</v>
+        <v>290618</v>
       </c>
       <c r="P3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Q3">
-        <v>34149.699999999997</v>
+        <v>372131</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="S3">
-        <v>25413</v>
+        <v>163358</v>
       </c>
       <c r="T3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="U3">
-        <v>29975.8</v>
+        <v>272524</v>
       </c>
       <c r="V3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="W3">
-        <v>34734.699999999997</v>
+        <v>328737</v>
       </c>
       <c r="X3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="Y3">
-        <v>24941</v>
+        <v>187296</v>
       </c>
       <c r="Z3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AA3">
-        <v>26625.7</v>
+        <v>173873</v>
       </c>
       <c r="AB3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="AC3">
-        <v>25825.7</v>
+        <v>189598</v>
       </c>
       <c r="AD3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AE3">
-        <v>17250.900000000001</v>
+        <v>35978</v>
       </c>
       <c r="AF3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="AG3">
-        <v>136036</v>
+        <v>176275</v>
       </c>
       <c r="AH3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AI3">
-        <v>50073.2</v>
+        <v>102247</v>
       </c>
       <c r="AJ3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="AK3">
-        <v>67205.3</v>
+        <v>122622</v>
       </c>
       <c r="AL3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AM3">
-        <v>119999</v>
+        <v>306649</v>
       </c>
       <c r="AN3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="AO3">
-        <v>74374</v>
+        <v>108984</v>
       </c>
       <c r="AP3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AQ3">
-        <v>79416.399999999994</v>
+        <v>178414</v>
       </c>
       <c r="AR3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AS3">
-        <v>1466.49</v>
+        <v>2237.0500000000002</v>
       </c>
       <c r="AT3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AU3">
-        <v>2846.11</v>
+        <v>4223.1499999999996</v>
       </c>
       <c r="AV3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AW3">
-        <v>9071.1299999999992</v>
+        <v>9368.52</v>
       </c>
       <c r="AX3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AY3">
-        <v>772.88</v>
+        <v>3536.26</v>
       </c>
       <c r="AZ3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="BA3">
-        <v>147738</v>
+        <v>292399</v>
       </c>
       <c r="BB3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="BC3">
-        <v>4383.28</v>
+        <v>4764.62</v>
       </c>
       <c r="BD3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="BE3">
-        <v>48980.7</v>
+        <v>53008.2</v>
       </c>
       <c r="BF3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1242,545 +1430,916 @@
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8730.19</v>
+        <v>7860.86</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C5">
-        <v>136256</v>
+        <v>129482</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E5">
-        <v>6877.8</v>
+        <v>6541.76</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G5">
-        <v>7140.21</v>
+        <v>7053.53</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I5">
-        <v>17459.2</v>
+        <v>17140</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K5">
-        <v>714.32299999999998</v>
+        <v>685.05</v>
       </c>
       <c r="L5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="M5">
-        <v>25049.9</v>
+        <v>23802.799999999999</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O5">
-        <v>31910.9</v>
+        <v>28208.6</v>
       </c>
       <c r="P5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q5">
-        <v>33371.599999999999</v>
+        <v>32529.1</v>
       </c>
       <c r="R5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="S5">
-        <v>24437.4</v>
+        <v>22988.799999999999</v>
       </c>
       <c r="T5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="U5">
-        <v>31153.4</v>
+        <v>27734.7</v>
       </c>
       <c r="V5" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="W5">
-        <v>34444.699999999997</v>
+        <v>32427.599999999999</v>
       </c>
       <c r="X5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="Y5">
-        <v>23723.599999999999</v>
+        <v>22197.1</v>
       </c>
       <c r="Z5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AA5">
-        <v>24674</v>
+        <v>22735.200000000001</v>
       </c>
       <c r="AB5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AC5">
-        <v>25713.4</v>
+        <v>23216.7</v>
       </c>
       <c r="AD5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AE5">
-        <v>16885</v>
+        <v>14917</v>
       </c>
       <c r="AF5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AG5">
-        <v>128439</v>
+        <v>110019</v>
       </c>
       <c r="AH5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AI5">
-        <v>51332.6</v>
+        <v>45333.2</v>
       </c>
       <c r="AJ5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AK5">
-        <v>74428.600000000006</v>
+        <v>61400.9</v>
       </c>
       <c r="AL5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AM5">
-        <v>112136</v>
+        <v>101484</v>
       </c>
       <c r="AN5" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AO5">
-        <v>75225.100000000006</v>
+        <v>66356.600000000006</v>
       </c>
       <c r="AP5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AQ5">
-        <v>88793.4</v>
+        <v>76476</v>
       </c>
       <c r="AR5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AS5">
-        <v>1336.01</v>
+        <v>1319.82</v>
       </c>
       <c r="AT5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AU5">
-        <v>2631.45</v>
+        <v>2585.69</v>
       </c>
       <c r="AV5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AW5">
-        <v>8818.9599999999991</v>
+        <v>8415.93</v>
       </c>
       <c r="AX5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="AY5">
-        <v>709.43700000000001</v>
+        <v>724.024</v>
       </c>
       <c r="AZ5" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="BA5">
-        <v>160814</v>
+        <v>140598</v>
       </c>
       <c r="BB5" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="BC5">
-        <v>4354.3599999999997</v>
+        <v>4272.83</v>
       </c>
       <c r="BD5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="BE5">
-        <v>51842.6</v>
+        <v>49756</v>
       </c>
       <c r="BF5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8457.35</v>
+        <v>8568.58</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C7">
-        <v>176578</v>
+        <v>140600</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E7">
-        <v>10326.200000000001</v>
+        <v>6902.58</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G7">
-        <v>12005.9</v>
+        <v>7475.43</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="I7">
-        <v>36002.9</v>
+        <v>17726.400000000001</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K7">
-        <v>791.73</v>
+        <v>706.40499999999997</v>
       </c>
       <c r="L7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M7">
-        <v>32760.6</v>
+        <v>23104.5</v>
       </c>
       <c r="N7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="O7">
-        <v>52248.5</v>
+        <v>30103.200000000001</v>
       </c>
       <c r="P7" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="Q7">
-        <v>64235.6</v>
+        <v>34539.300000000003</v>
       </c>
       <c r="R7" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="S7">
-        <v>36783.5</v>
+        <v>25410</v>
       </c>
       <c r="T7" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="U7">
-        <v>55177.5</v>
+        <v>29326.2</v>
       </c>
       <c r="V7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="W7">
-        <v>72954.5</v>
+        <v>34909.199999999997</v>
       </c>
       <c r="X7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="Y7">
-        <v>35626</v>
+        <v>24176.2</v>
       </c>
       <c r="Z7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AA7">
-        <v>34502.199999999997</v>
+        <v>24490.5</v>
       </c>
       <c r="AB7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="AC7">
-        <v>35015</v>
+        <v>25596</v>
       </c>
       <c r="AD7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="AE7">
-        <v>23410.799999999999</v>
+        <v>16758.099999999999</v>
       </c>
       <c r="AF7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="AG7">
-        <v>145002</v>
+        <v>114804</v>
       </c>
       <c r="AH7" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="AI7">
-        <v>135408</v>
+        <v>47137.4</v>
       </c>
       <c r="AJ7" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="AK7">
-        <v>135819</v>
+        <v>63665.7</v>
       </c>
       <c r="AL7" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AM7">
-        <v>160541</v>
+        <v>101522</v>
       </c>
       <c r="AN7" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AO7">
-        <v>182558</v>
+        <v>61675.3</v>
       </c>
       <c r="AP7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AQ7">
-        <v>208298</v>
+        <v>79877.2</v>
       </c>
       <c r="AR7" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AS7">
-        <v>1658.12</v>
+        <v>1340.2</v>
       </c>
       <c r="AT7" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AU7">
-        <v>4184.17</v>
+        <v>2631.45</v>
       </c>
       <c r="AV7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AW7">
-        <v>12704.8</v>
+        <v>9371.8799999999992</v>
       </c>
       <c r="AX7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AY7">
-        <v>850.53800000000001</v>
+        <v>751.91800000000001</v>
       </c>
       <c r="AZ7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="BA7">
-        <v>321083</v>
+        <v>149290</v>
       </c>
       <c r="BB7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="BC7">
-        <v>7967.06</v>
+        <v>4364.37</v>
       </c>
       <c r="BD7" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="BE7">
-        <v>91064.8</v>
+        <v>50042.7</v>
       </c>
       <c r="BF7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>9196.7999999999993</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9">
+        <v>170135</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9">
+        <v>8570.57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9">
+        <v>9392.58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>132</v>
+      </c>
+      <c r="I9">
+        <v>26107.200000000001</v>
+      </c>
+      <c r="J9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K9">
+        <v>900.46100000000001</v>
+      </c>
+      <c r="L9" t="s">
+        <v>134</v>
+      </c>
+      <c r="M9">
+        <v>29557.5</v>
+      </c>
+      <c r="N9" t="s">
+        <v>135</v>
+      </c>
+      <c r="O9">
+        <v>45719.4</v>
+      </c>
+      <c r="P9" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q9">
+        <v>66670.5</v>
+      </c>
+      <c r="R9" t="s">
+        <v>137</v>
+      </c>
+      <c r="S9">
+        <v>31799.4</v>
+      </c>
+      <c r="T9" t="s">
+        <v>138</v>
+      </c>
+      <c r="U9">
+        <v>58402.1</v>
+      </c>
+      <c r="V9" t="s">
+        <v>139</v>
+      </c>
+      <c r="W9">
+        <v>61023.1</v>
+      </c>
+      <c r="X9" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y9">
+        <v>33507.599999999999</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA9">
+        <v>32925.9</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC9">
+        <v>32892</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE9">
+        <v>21754.3</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG9">
+        <v>156732</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI9">
+        <v>108680</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK9">
+        <v>132347</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM9">
+        <v>174101</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>148</v>
+      </c>
+      <c r="AO9">
+        <v>189207</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AQ9">
+        <v>230445</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>150</v>
+      </c>
+      <c r="AS9">
+        <v>1562.43</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>151</v>
+      </c>
+      <c r="AU9">
+        <v>4166.6099999999997</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>152</v>
+      </c>
+      <c r="AW9">
+        <v>11014.9</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>153</v>
+      </c>
+      <c r="AY9">
+        <v>1020.18</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>154</v>
+      </c>
+      <c r="BA9">
+        <v>307810</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>155</v>
+      </c>
+      <c r="BC9">
+        <v>6158.34</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>156</v>
+      </c>
+      <c r="BE9">
+        <v>73013.2</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9162.8700000000008</v>
+      </c>
+      <c r="B11" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11">
+        <v>141607</v>
+      </c>
+      <c r="D11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11">
+        <v>7497.62</v>
+      </c>
+      <c r="F11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G11">
+        <v>8222.15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11">
+        <v>18363.599999999999</v>
+      </c>
+      <c r="J11" t="s">
+        <v>164</v>
+      </c>
+      <c r="K11">
+        <v>810.07</v>
+      </c>
+      <c r="L11" t="s">
+        <v>165</v>
+      </c>
+      <c r="M11">
+        <v>27018.3</v>
+      </c>
+      <c r="N11" t="s">
+        <v>166</v>
+      </c>
+      <c r="O11">
+        <v>33177.4</v>
+      </c>
+      <c r="P11" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q11">
+        <v>36051.599999999999</v>
+      </c>
+      <c r="R11" t="s">
+        <v>168</v>
+      </c>
+      <c r="S11">
+        <v>27490.9</v>
+      </c>
+      <c r="T11" t="s">
+        <v>169</v>
+      </c>
+      <c r="U11">
+        <v>36466.1</v>
+      </c>
+      <c r="V11" t="s">
+        <v>170</v>
+      </c>
+      <c r="W11">
+        <v>38311.4</v>
+      </c>
+      <c r="X11" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y11">
+        <v>25138.799999999999</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA11">
+        <v>27874.2</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC11">
+        <v>28374.3</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE11">
+        <v>19425.8</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG11">
+        <v>86247.3</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI11">
+        <v>53182.8</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK11">
+        <v>70596.899999999994</v>
+      </c>
+      <c r="AL11" t="s">
+        <v>178</v>
+      </c>
+      <c r="AM11">
+        <v>124714</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>179</v>
+      </c>
+      <c r="AO11">
+        <v>64525.5</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ11">
+        <v>50642.3</v>
+      </c>
+      <c r="AR11" t="s">
+        <v>181</v>
+      </c>
+      <c r="AS11">
+        <v>1475.8</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AU11">
+        <v>2823.35</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AW11">
+        <v>10039.6</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>184</v>
+      </c>
+      <c r="AY11">
+        <v>852.27099999999996</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA11">
+        <v>151669</v>
+      </c>
+      <c r="BB11" t="s">
+        <v>186</v>
+      </c>
+      <c r="BC11">
+        <v>4946.16</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>187</v>
+      </c>
+      <c r="BE11">
+        <v>50656.3</v>
+      </c>
+      <c r="BF11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>7542</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>118282</v>
       </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>6110</v>
       </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>6528</v>
       </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9">
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13">
         <v>15780</v>
       </c>
-      <c r="J9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9">
+      <c r="J13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13">
         <v>629</v>
       </c>
-      <c r="L9" t="s">
-        <v>1</v>
-      </c>
-      <c r="M9">
+      <c r="L13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13">
         <v>21282</v>
       </c>
-      <c r="N9" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9">
+      <c r="N13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13">
         <v>26524</v>
       </c>
-      <c r="P9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q9">
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13">
         <v>29368</v>
       </c>
-      <c r="R9" t="s">
-        <v>1</v>
-      </c>
-      <c r="S9">
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13">
         <v>22141</v>
       </c>
-      <c r="T9" t="s">
-        <v>1</v>
-      </c>
-      <c r="U9">
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13">
         <v>26130</v>
       </c>
-      <c r="V9" t="s">
-        <v>1</v>
-      </c>
-      <c r="W9">
+      <c r="V13" t="s">
+        <v>1</v>
+      </c>
+      <c r="W13">
         <v>29437</v>
       </c>
-      <c r="X9" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y9">
+      <c r="X13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y13">
         <v>20749</v>
       </c>
-      <c r="Z9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA9">
+      <c r="Z13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA13">
         <v>21294</v>
       </c>
-      <c r="AB9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC9">
+      <c r="AB13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC13">
         <v>22068</v>
       </c>
-      <c r="AD9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE9">
+      <c r="AD13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE13">
         <v>14379</v>
       </c>
-      <c r="AF9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG9">
+      <c r="AF13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG13">
         <v>108059</v>
       </c>
-      <c r="AH9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI9">
+      <c r="AH13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI13">
         <v>44303</v>
       </c>
-      <c r="AJ9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK9">
+      <c r="AJ13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK13">
         <v>59030</v>
       </c>
-      <c r="AL9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM9">
+      <c r="AL13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM13">
         <v>96772</v>
       </c>
-      <c r="AN9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO9">
+      <c r="AN13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO13">
         <v>58537</v>
       </c>
-      <c r="AP9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ9">
+      <c r="AP13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ13">
         <v>73682</v>
       </c>
-      <c r="AR9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS9">
+      <c r="AR13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS13">
         <v>1211</v>
       </c>
-      <c r="AT9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU9">
+      <c r="AT13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU13">
         <v>2323</v>
       </c>
-      <c r="AV9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW9">
+      <c r="AV13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW13">
         <v>7910</v>
       </c>
-      <c r="AX9" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY9">
+      <c r="AX13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY13">
         <v>675</v>
       </c>
-      <c r="AZ9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA9">
+      <c r="AZ13" t="s">
+        <v>1</v>
+      </c>
+      <c r="BA13">
         <v>126643</v>
       </c>
-      <c r="BB9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BC9">
+      <c r="BB13" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC13">
         <v>3916</v>
       </c>
-      <c r="BD9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BE9">
+      <c r="BD13" t="s">
+        <v>1</v>
+      </c>
+      <c r="BE13">
         <v>42080</v>
       </c>
-      <c r="BF9" t="s">
+      <c r="BF13" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
set -o3 compile & optimize Ant
</commit_message>
<xml_diff>
--- a/TSP/output.xlsx
+++ b/TSP/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA12879-1A73-41AA-A540-4E9CE43AB31D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77644883-8B50-457F-B491-68F34614B163}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{17DF2899-9B80-469F-8091-A3CD22A51120}" name="briefOutput" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="936" sourceFile="C:\Users\66919\TSP-Course-Design\TSP\briefOutput.txt" tab="0" space="1" consecutive="1">
+  <connection id="1" xr16:uid="{EDD029B1-C12B-4BD7-9056-7A56060184B7}" name="briefOutput" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="936" sourceFile="C:\Users\66919\TSP-Course-Design\TSP\briefOutput.txt" space="1" consecutive="1">
       <textFields count="58">
         <textField/>
         <textField/>
@@ -220,445 +220,445 @@
     <t>Crowd</t>
   </si>
   <si>
-    <t>5260.4ms</t>
-  </si>
-  <si>
-    <t>5347.66ms</t>
-  </si>
-  <si>
-    <t>4767.14ms</t>
-  </si>
-  <si>
-    <t>4733.98ms</t>
-  </si>
-  <si>
-    <t>3949.2ms</t>
-  </si>
-  <si>
-    <t>4313.67ms</t>
-  </si>
-  <si>
-    <t>4310.25ms</t>
-  </si>
-  <si>
-    <t>4338.98ms</t>
-  </si>
-  <si>
-    <t>4259.5ms</t>
-  </si>
-  <si>
-    <t>4284.98ms</t>
-  </si>
-  <si>
-    <t>4370.26ms</t>
-  </si>
-  <si>
-    <t>4249.29ms</t>
-  </si>
-  <si>
-    <t>4180.57ms</t>
-  </si>
-  <si>
-    <t>4236.35ms</t>
-  </si>
-  <si>
-    <t>4236.66ms</t>
-  </si>
-  <si>
-    <t>4241.68ms</t>
-  </si>
-  <si>
-    <t>4284.78ms</t>
-  </si>
-  <si>
-    <t>4422.44ms</t>
-  </si>
-  <si>
-    <t>4293.66ms</t>
-  </si>
-  <si>
-    <t>6219.8ms</t>
-  </si>
-  <si>
-    <t>4295.97ms</t>
-  </si>
-  <si>
-    <t>4348.34ms</t>
-  </si>
-  <si>
-    <t>4279.7ms</t>
-  </si>
-  <si>
-    <t>4259.25ms</t>
-  </si>
-  <si>
-    <t>4121.73ms</t>
-  </si>
-  <si>
-    <t>4271.65ms</t>
-  </si>
-  <si>
-    <t>4252.07ms</t>
-  </si>
-  <si>
-    <t>3815.7ms</t>
-  </si>
-  <si>
-    <t>4480.63ms</t>
-  </si>
-  <si>
-    <t>0.1803ms</t>
-  </si>
-  <si>
-    <t>0.9803ms</t>
-  </si>
-  <si>
-    <t>1.1154ms</t>
-  </si>
-  <si>
-    <t>1.2861ms</t>
-  </si>
-  <si>
-    <t>2.1791ms</t>
-  </si>
-  <si>
-    <t>0.6375ms</t>
-  </si>
-  <si>
-    <t>0.704ms</t>
-  </si>
-  <si>
-    <t>1.4015ms</t>
-  </si>
-  <si>
-    <t>4.9262ms</t>
-  </si>
-  <si>
-    <t>0.6377ms</t>
-  </si>
-  <si>
-    <t>1.789ms</t>
-  </si>
-  <si>
-    <t>2.3914ms</t>
+    <t>Algo4:</t>
+  </si>
+  <si>
+    <t>greedyKNN</t>
   </si>
   <si>
     <t>0.6278ms</t>
   </si>
   <si>
-    <t>0.7888ms</t>
-  </si>
-  <si>
-    <t>0.7142ms</t>
-  </si>
-  <si>
-    <t>0.7259ms</t>
-  </si>
-  <si>
-    <t>0.3744ms</t>
-  </si>
-  <si>
-    <t>0.7234ms</t>
-  </si>
-  <si>
-    <t>1.4656ms</t>
-  </si>
-  <si>
-    <t>1.1267ms</t>
-  </si>
-  <si>
-    <t>1.2605ms</t>
-  </si>
-  <si>
-    <t>1.6016ms</t>
-  </si>
-  <si>
-    <t>0.6103ms</t>
-  </si>
-  <si>
-    <t>3.2973ms</t>
-  </si>
-  <si>
-    <t>0.7731ms</t>
-  </si>
-  <si>
-    <t>0.3182ms</t>
-  </si>
-  <si>
-    <t>2.9669ms</t>
-  </si>
-  <si>
-    <t>2.9109ms</t>
-  </si>
-  <si>
-    <t>1.4607ms</t>
-  </si>
-  <si>
-    <t>0.1581ms</t>
-  </si>
-  <si>
-    <t>0.931ms</t>
-  </si>
-  <si>
-    <t>1.2971ms</t>
-  </si>
-  <si>
-    <t>1.27ms</t>
-  </si>
-  <si>
-    <t>2.0017ms</t>
-  </si>
-  <si>
-    <t>0.6252ms</t>
-  </si>
-  <si>
-    <t>0.6266ms</t>
-  </si>
-  <si>
-    <t>1.41ms</t>
-  </si>
-  <si>
-    <t>3.3162ms</t>
-  </si>
-  <si>
-    <t>0.6578ms</t>
-  </si>
-  <si>
-    <t>1.4763ms</t>
-  </si>
-  <si>
-    <t>2.9671ms</t>
-  </si>
-  <si>
-    <t>0.6566ms</t>
-  </si>
-  <si>
-    <t>0.7343ms</t>
-  </si>
-  <si>
-    <t>1.0932ms</t>
-  </si>
-  <si>
-    <t>0.7136ms</t>
-  </si>
-  <si>
-    <t>0.4837ms</t>
-  </si>
-  <si>
-    <t>0.758ms</t>
-  </si>
-  <si>
-    <t>1.2284ms</t>
-  </si>
-  <si>
-    <t>1.6024ms</t>
-  </si>
-  <si>
-    <t>1.3456ms</t>
-  </si>
-  <si>
-    <t>2.1371ms</t>
-  </si>
-  <si>
-    <t>0.7166ms</t>
-  </si>
-  <si>
-    <t>2.2502ms</t>
-  </si>
-  <si>
-    <t>0.6579ms</t>
-  </si>
-  <si>
-    <t>0.3425ms</t>
-  </si>
-  <si>
-    <t>2.9906ms</t>
-  </si>
-  <si>
-    <t>2.6189ms</t>
-  </si>
-  <si>
-    <t>1.8839ms</t>
-  </si>
-  <si>
-    <t>126.888ms</t>
-  </si>
-  <si>
-    <t>485.986ms</t>
-  </si>
-  <si>
-    <t>1977.38ms</t>
-  </si>
-  <si>
-    <t>2886.31ms</t>
-  </si>
-  <si>
-    <t>6740.94ms</t>
-  </si>
-  <si>
-    <t>359.45ms</t>
-  </si>
-  <si>
-    <t>364.947ms</t>
-  </si>
-  <si>
-    <t>566.964ms</t>
-  </si>
-  <si>
-    <t>713.717ms</t>
-  </si>
-  <si>
-    <t>361.662ms</t>
-  </si>
-  <si>
-    <t>532.448ms</t>
-  </si>
-  <si>
-    <t>768.943ms</t>
-  </si>
-  <si>
-    <t>376.425ms</t>
-  </si>
-  <si>
-    <t>375.237ms</t>
-  </si>
-  <si>
-    <t>363.154ms</t>
-  </si>
-  <si>
-    <t>394.485ms</t>
-  </si>
-  <si>
-    <t>278.569ms</t>
-  </si>
-  <si>
-    <t>389.051ms</t>
-  </si>
-  <si>
-    <t>445.433ms</t>
-  </si>
-  <si>
-    <t>490.126ms</t>
-  </si>
-  <si>
-    <t>521.68ms</t>
-  </si>
-  <si>
-    <t>543.499ms</t>
-  </si>
-  <si>
-    <t>356.403ms</t>
-  </si>
-  <si>
-    <t>688.488ms</t>
-  </si>
-  <si>
-    <t>881.531ms</t>
-  </si>
-  <si>
-    <t>289.399ms</t>
-  </si>
-  <si>
-    <t>800.752ms</t>
-  </si>
-  <si>
-    <t>11739.9ms</t>
-  </si>
-  <si>
-    <t>3141.41ms</t>
-  </si>
-  <si>
-    <t>Algo4:</t>
-  </si>
-  <si>
-    <t>greedyKNN</t>
-  </si>
-  <si>
-    <t>0.1301ms</t>
-  </si>
-  <si>
-    <t>1.6658ms</t>
-  </si>
-  <si>
-    <t>1.7893ms</t>
-  </si>
-  <si>
-    <t>2.6644ms</t>
-  </si>
-  <si>
-    <t>6.0405ms</t>
-  </si>
-  <si>
-    <t>0.8405ms</t>
-  </si>
-  <si>
-    <t>0.8275ms</t>
-  </si>
-  <si>
-    <t>4.1504ms</t>
-  </si>
-  <si>
-    <t>6.1197ms</t>
-  </si>
-  <si>
-    <t>0.871ms</t>
-  </si>
-  <si>
-    <t>2.7986ms</t>
-  </si>
-  <si>
-    <t>7.0579ms</t>
-  </si>
-  <si>
-    <t>1.0396ms</t>
-  </si>
-  <si>
-    <t>0.9319ms</t>
-  </si>
-  <si>
-    <t>0.825ms</t>
-  </si>
-  <si>
-    <t>0.9345ms</t>
-  </si>
-  <si>
-    <t>0.4019ms</t>
-  </si>
-  <si>
-    <t>1.2669ms</t>
-  </si>
-  <si>
-    <t>1.6327ms</t>
-  </si>
-  <si>
-    <t>1.9897ms</t>
-  </si>
-  <si>
-    <t>2.6261ms</t>
-  </si>
-  <si>
-    <t>2.8253ms</t>
-  </si>
-  <si>
-    <t>0.7843ms</t>
-  </si>
-  <si>
-    <t>5.9286ms</t>
-  </si>
-  <si>
-    <t>0.847ms</t>
-  </si>
-  <si>
-    <t>0.3195ms</t>
-  </si>
-  <si>
-    <t>9.6308ms</t>
-  </si>
-  <si>
-    <t>8.9106ms</t>
-  </si>
-  <si>
-    <t>3.2304ms</t>
+    <t>0.0773ms</t>
+  </si>
+  <si>
+    <t>0.24ms</t>
+  </si>
+  <si>
+    <t>0.2656ms</t>
+  </si>
+  <si>
+    <t>0.513ms</t>
+  </si>
+  <si>
+    <t>0.203ms</t>
+  </si>
+  <si>
+    <t>0.3348ms</t>
+  </si>
+  <si>
+    <t>0.5374ms</t>
+  </si>
+  <si>
+    <t>0.7656ms</t>
+  </si>
+  <si>
+    <t>0.1862ms</t>
+  </si>
+  <si>
+    <t>0.5446ms</t>
+  </si>
+  <si>
+    <t>0.7659ms</t>
+  </si>
+  <si>
+    <t>0.1876ms</t>
+  </si>
+  <si>
+    <t>0.3433ms</t>
+  </si>
+  <si>
+    <t>0.3442ms</t>
+  </si>
+  <si>
+    <t>0.3552ms</t>
+  </si>
+  <si>
+    <t>0.295ms</t>
+  </si>
+  <si>
+    <t>0.3752ms</t>
+  </si>
+  <si>
+    <t>0.479ms</t>
+  </si>
+  <si>
+    <t>0.4843ms</t>
+  </si>
+  <si>
+    <t>0.3748ms</t>
+  </si>
+  <si>
+    <t>0.5872ms</t>
+  </si>
+  <si>
+    <t>0.2976ms</t>
+  </si>
+  <si>
+    <t>0.4932ms</t>
+  </si>
+  <si>
+    <t>0.3506ms</t>
+  </si>
+  <si>
+    <t>0.1189ms</t>
+  </si>
+  <si>
+    <t>0.8219ms</t>
+  </si>
+  <si>
+    <t>0.6113ms</t>
+  </si>
+  <si>
+    <t>0.6935ms</t>
+  </si>
+  <si>
+    <t>0.2449ms</t>
+  </si>
+  <si>
+    <t>0.5123ms</t>
+  </si>
+  <si>
+    <t>0.5204ms</t>
+  </si>
+  <si>
+    <t>0.6102ms</t>
+  </si>
+  <si>
+    <t>0.7917ms</t>
+  </si>
+  <si>
+    <t>0.4224ms</t>
+  </si>
+  <si>
+    <t>0.3648ms</t>
+  </si>
+  <si>
+    <t>0.6529ms</t>
+  </si>
+  <si>
+    <t>0.8174ms</t>
+  </si>
+  <si>
+    <t>0.4199ms</t>
+  </si>
+  <si>
+    <t>0.5957ms</t>
+  </si>
+  <si>
+    <t>0.8556ms</t>
+  </si>
+  <si>
+    <t>0.2974ms</t>
+  </si>
+  <si>
+    <t>0.4163ms</t>
+  </si>
+  <si>
+    <t>0.3411ms</t>
+  </si>
+  <si>
+    <t>0.4753ms</t>
+  </si>
+  <si>
+    <t>0.2563ms</t>
+  </si>
+  <si>
+    <t>0.4214ms</t>
+  </si>
+  <si>
+    <t>0.5014ms</t>
+  </si>
+  <si>
+    <t>0.505ms</t>
+  </si>
+  <si>
+    <t>0.6175ms</t>
+  </si>
+  <si>
+    <t>0.5916ms</t>
+  </si>
+  <si>
+    <t>0.4209ms</t>
+  </si>
+  <si>
+    <t>0.7505ms</t>
+  </si>
+  <si>
+    <t>0.3998ms</t>
+  </si>
+  <si>
+    <t>0.3234ms</t>
+  </si>
+  <si>
+    <t>1.0363ms</t>
+  </si>
+  <si>
+    <t>0.8073ms</t>
+  </si>
+  <si>
+    <t>0.6666ms</t>
+  </si>
+  <si>
+    <t>38.7741ms</t>
+  </si>
+  <si>
+    <t>138.693ms</t>
+  </si>
+  <si>
+    <t>619.095ms</t>
+  </si>
+  <si>
+    <t>951.474ms</t>
+  </si>
+  <si>
+    <t>2236.4ms</t>
+  </si>
+  <si>
+    <t>109.749ms</t>
+  </si>
+  <si>
+    <t>113.266ms</t>
+  </si>
+  <si>
+    <t>160.213ms</t>
+  </si>
+  <si>
+    <t>211.845ms</t>
+  </si>
+  <si>
+    <t>109.561ms</t>
+  </si>
+  <si>
+    <t>159.985ms</t>
+  </si>
+  <si>
+    <t>210.001ms</t>
+  </si>
+  <si>
+    <t>113.835ms</t>
+  </si>
+  <si>
+    <t>109.478ms</t>
+  </si>
+  <si>
+    <t>108.633ms</t>
+  </si>
+  <si>
+    <t>113.225ms</t>
+  </si>
+  <si>
+    <t>87.9876ms</t>
+  </si>
+  <si>
+    <t>116.821ms</t>
+  </si>
+  <si>
+    <t>133.375ms</t>
+  </si>
+  <si>
+    <t>145.546ms</t>
+  </si>
+  <si>
+    <t>158.389ms</t>
+  </si>
+  <si>
+    <t>169.551ms</t>
+  </si>
+  <si>
+    <t>107.31ms</t>
+  </si>
+  <si>
+    <t>206.743ms</t>
+  </si>
+  <si>
+    <t>278.173ms</t>
+  </si>
+  <si>
+    <t>80.0004ms</t>
+  </si>
+  <si>
+    <t>236.053ms</t>
+  </si>
+  <si>
+    <t>3145.56ms</t>
+  </si>
+  <si>
+    <t>1067.52ms</t>
+  </si>
+  <si>
+    <t>0.1016ms</t>
+  </si>
+  <si>
+    <t>0.5019ms</t>
+  </si>
+  <si>
+    <t>0.5173ms</t>
+  </si>
+  <si>
+    <t>0.8785ms</t>
+  </si>
+  <si>
+    <t>1.3006ms</t>
+  </si>
+  <si>
+    <t>0.3046ms</t>
+  </si>
+  <si>
+    <t>0.3289ms</t>
+  </si>
+  <si>
+    <t>0.7124ms</t>
+  </si>
+  <si>
+    <t>1.3589ms</t>
+  </si>
+  <si>
+    <t>0.3077ms</t>
+  </si>
+  <si>
+    <t>0.7242ms</t>
+  </si>
+  <si>
+    <t>1.3894ms</t>
+  </si>
+  <si>
+    <t>0.2927ms</t>
+  </si>
+  <si>
+    <t>0.2814ms</t>
+  </si>
+  <si>
+    <t>0.2884ms</t>
+  </si>
+  <si>
+    <t>0.3302ms</t>
+  </si>
+  <si>
+    <t>0.1579ms</t>
+  </si>
+  <si>
+    <t>0.3048ms</t>
+  </si>
+  <si>
+    <t>0.4525ms</t>
+  </si>
+  <si>
+    <t>0.5629ms</t>
+  </si>
+  <si>
+    <t>0.5987ms</t>
+  </si>
+  <si>
+    <t>0.6384ms</t>
+  </si>
+  <si>
+    <t>0.271ms</t>
+  </si>
+  <si>
+    <t>1.2695ms</t>
+  </si>
+  <si>
+    <t>0.2381ms</t>
+  </si>
+  <si>
+    <t>0.1202ms</t>
+  </si>
+  <si>
+    <t>1.8599ms</t>
+  </si>
+  <si>
+    <t>1.7496ms</t>
+  </si>
+  <si>
+    <t>0.726ms</t>
+  </si>
+  <si>
+    <t>46.1801ms</t>
+  </si>
+  <si>
+    <t>469.635ms</t>
+  </si>
+  <si>
+    <t>532.303ms</t>
+  </si>
+  <si>
+    <t>797.488ms</t>
+  </si>
+  <si>
+    <t>1347.59ms</t>
+  </si>
+  <si>
+    <t>244.373ms</t>
+  </si>
+  <si>
+    <t>243.846ms</t>
+  </si>
+  <si>
+    <t>761.285ms</t>
+  </si>
+  <si>
+    <t>1729.06ms</t>
+  </si>
+  <si>
+    <t>242.464ms</t>
+  </si>
+  <si>
+    <t>760.592ms</t>
+  </si>
+  <si>
+    <t>1732.77ms</t>
+  </si>
+  <si>
+    <t>242.709ms</t>
+  </si>
+  <si>
+    <t>243.948ms</t>
+  </si>
+  <si>
+    <t>247.149ms</t>
+  </si>
+  <si>
+    <t>278.23ms</t>
+  </si>
+  <si>
+    <t>110.281ms</t>
+  </si>
+  <si>
+    <t>294.345ms</t>
+  </si>
+  <si>
+    <t>449.905ms</t>
+  </si>
+  <si>
+    <t>573.458ms</t>
+  </si>
+  <si>
+    <t>682.644ms</t>
+  </si>
+  <si>
+    <t>797.608ms</t>
+  </si>
+  <si>
+    <t>235.719ms</t>
+  </si>
+  <si>
+    <t>1607.56ms</t>
+  </si>
+  <si>
+    <t>271.713ms</t>
+  </si>
+  <si>
+    <t>90.8842ms</t>
+  </si>
+  <si>
+    <t>2478.03ms</t>
+  </si>
+  <si>
+    <t>2003.2ms</t>
+  </si>
+  <si>
+    <t>705.732ms</t>
   </si>
 </sst>
 </file>
@@ -721,7 +721,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="briefOutput_1" connectionId="1" xr16:uid="{FEBA5FEE-30F3-4377-9FD9-21063A689EC8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="briefOutput_1" connectionId="1" xr16:uid="{7EF389AB-0BCD-4BFC-9145-9BB1D2DB65D5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -990,7 +990,7 @@
   <dimension ref="A1:BF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1026,7 @@
     <col min="30" max="30" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -1232,197 +1232,197 @@
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8511.58</v>
+        <v>7860.86</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>408478</v>
+        <v>129482</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E3">
-        <v>6965.39</v>
+        <v>6541.76</v>
       </c>
       <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>7053.53</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3">
+        <v>17140</v>
+      </c>
+      <c r="J3" t="s">
         <v>44</v>
       </c>
-      <c r="G3">
-        <v>7534.85</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3">
-        <v>17867</v>
-      </c>
-      <c r="J3" t="s">
-        <v>46</v>
-      </c>
       <c r="K3">
-        <v>2142.5300000000002</v>
+        <v>685.05</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M3">
-        <v>182798</v>
+        <v>23802.799999999999</v>
       </c>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O3">
-        <v>290618</v>
+        <v>28208.6</v>
       </c>
       <c r="P3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Q3">
-        <v>372131</v>
+        <v>32529.1</v>
       </c>
       <c r="R3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S3">
-        <v>163358</v>
+        <v>22988.799999999999</v>
       </c>
       <c r="T3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="U3">
-        <v>272524</v>
+        <v>27734.7</v>
       </c>
       <c r="V3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="W3">
-        <v>328737</v>
+        <v>32427.599999999999</v>
       </c>
       <c r="X3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Y3">
-        <v>187296</v>
+        <v>22197.1</v>
       </c>
       <c r="Z3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AA3">
-        <v>173873</v>
+        <v>22735.200000000001</v>
       </c>
       <c r="AB3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AC3">
-        <v>189598</v>
+        <v>23216.7</v>
       </c>
       <c r="AD3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AE3">
-        <v>35978</v>
+        <v>14917</v>
       </c>
       <c r="AF3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AG3">
-        <v>176275</v>
+        <v>110019</v>
       </c>
       <c r="AH3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AI3">
-        <v>102247</v>
+        <v>45333.2</v>
       </c>
       <c r="AJ3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AK3">
-        <v>122622</v>
+        <v>61400.9</v>
       </c>
       <c r="AL3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AM3">
-        <v>306649</v>
+        <v>101484</v>
       </c>
       <c r="AN3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AO3">
-        <v>108984</v>
+        <v>66356.600000000006</v>
       </c>
       <c r="AP3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AQ3">
-        <v>178414</v>
+        <v>76476</v>
       </c>
       <c r="AR3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AS3">
-        <v>2237.0500000000002</v>
+        <v>1319.82</v>
       </c>
       <c r="AT3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="AU3">
-        <v>4223.1499999999996</v>
+        <v>2585.69</v>
       </c>
       <c r="AV3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="AW3">
-        <v>9368.52</v>
+        <v>8415.93</v>
       </c>
       <c r="AX3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AY3">
-        <v>3536.26</v>
+        <v>724.024</v>
       </c>
       <c r="AZ3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="BA3">
-        <v>292399</v>
+        <v>140598</v>
       </c>
       <c r="BB3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="BC3">
-        <v>4764.62</v>
+        <v>4272.83</v>
       </c>
       <c r="BD3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="BE3">
-        <v>53008.2</v>
+        <v>49756</v>
       </c>
       <c r="BF3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -1430,733 +1430,733 @@
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>7860.86</v>
+        <v>8568.58</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C5">
-        <v>129482</v>
+        <v>140600</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E5">
-        <v>6541.76</v>
+        <v>6902.58</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G5">
-        <v>7053.53</v>
+        <v>7475.43</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I5">
-        <v>17140</v>
+        <v>17726.400000000001</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K5">
-        <v>685.05</v>
+        <v>706.40499999999997</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M5">
-        <v>23802.799999999999</v>
+        <v>23104.5</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="O5">
-        <v>28208.6</v>
+        <v>30103.200000000001</v>
       </c>
       <c r="P5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q5">
-        <v>32529.1</v>
+        <v>34539.300000000003</v>
       </c>
       <c r="R5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="S5">
-        <v>22988.799999999999</v>
+        <v>25410</v>
       </c>
       <c r="T5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="U5">
-        <v>27734.7</v>
+        <v>29326.2</v>
       </c>
       <c r="V5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="W5">
-        <v>32427.599999999999</v>
+        <v>34909.199999999997</v>
       </c>
       <c r="X5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Y5">
-        <v>22197.1</v>
+        <v>24176.2</v>
       </c>
       <c r="Z5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="AA5">
-        <v>22735.200000000001</v>
+        <v>24490.5</v>
       </c>
       <c r="AB5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="AC5">
-        <v>23216.7</v>
+        <v>25596</v>
       </c>
       <c r="AD5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AE5">
-        <v>14917</v>
+        <v>16758.099999999999</v>
       </c>
       <c r="AF5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AG5">
-        <v>110019</v>
+        <v>114804</v>
       </c>
       <c r="AH5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="AI5">
-        <v>45333.2</v>
+        <v>47137.4</v>
       </c>
       <c r="AJ5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="AK5">
-        <v>61400.9</v>
+        <v>63665.7</v>
       </c>
       <c r="AL5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="AM5">
-        <v>101484</v>
+        <v>101522</v>
       </c>
       <c r="AN5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AO5">
-        <v>66356.600000000006</v>
+        <v>61675.3</v>
       </c>
       <c r="AP5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AQ5">
-        <v>76476</v>
+        <v>79877.2</v>
       </c>
       <c r="AR5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="AS5">
-        <v>1319.82</v>
+        <v>1340.2</v>
       </c>
       <c r="AT5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AU5">
-        <v>2585.69</v>
+        <v>2631.45</v>
       </c>
       <c r="AV5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AW5">
-        <v>8415.93</v>
+        <v>9371.8799999999992</v>
       </c>
       <c r="AX5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AY5">
-        <v>724.024</v>
+        <v>751.91800000000001</v>
       </c>
       <c r="AZ5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="BA5">
-        <v>140598</v>
+        <v>149290</v>
       </c>
       <c r="BB5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="BC5">
-        <v>4272.83</v>
+        <v>4364.37</v>
       </c>
       <c r="BD5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="BE5">
-        <v>49756</v>
+        <v>50042.7</v>
       </c>
       <c r="BF5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>8568.58</v>
+        <v>9012.4699999999993</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C7">
-        <v>140600</v>
+        <v>171206</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E7">
-        <v>6902.58</v>
+        <v>8104.27</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G7">
-        <v>7475.43</v>
+        <v>9526.4500000000007</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I7">
-        <v>17726.400000000001</v>
+        <v>30688.9</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K7">
-        <v>706.40499999999997</v>
+        <v>860.43399999999997</v>
       </c>
       <c r="L7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="M7">
-        <v>23104.5</v>
+        <v>31594.7</v>
       </c>
       <c r="N7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="O7">
-        <v>30103.200000000001</v>
+        <v>51234.7</v>
       </c>
       <c r="P7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q7">
-        <v>34539.300000000003</v>
+        <v>62149.7</v>
       </c>
       <c r="R7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="S7">
-        <v>25410</v>
+        <v>38049.199999999997</v>
       </c>
       <c r="T7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="U7">
-        <v>29326.2</v>
+        <v>46315.6</v>
       </c>
       <c r="V7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="W7">
-        <v>34909.199999999997</v>
+        <v>73704</v>
       </c>
       <c r="X7" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="Y7">
-        <v>24176.2</v>
+        <v>31801.200000000001</v>
       </c>
       <c r="Z7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="AA7">
-        <v>24490.5</v>
+        <v>37174.1</v>
       </c>
       <c r="AB7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="AC7">
-        <v>25596</v>
+        <v>37989.300000000003</v>
       </c>
       <c r="AD7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="AE7">
-        <v>16758.099999999999</v>
+        <v>22025.8</v>
       </c>
       <c r="AF7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="AG7">
-        <v>114804</v>
+        <v>141913</v>
       </c>
       <c r="AH7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="AI7">
-        <v>47137.4</v>
+        <v>152537</v>
       </c>
       <c r="AJ7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="AK7">
-        <v>63665.7</v>
+        <v>133728</v>
       </c>
       <c r="AL7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="AM7">
-        <v>101522</v>
+        <v>161166</v>
       </c>
       <c r="AN7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="AO7">
-        <v>61675.3</v>
+        <v>168217</v>
       </c>
       <c r="AP7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="AQ7">
-        <v>79877.2</v>
+        <v>235819</v>
       </c>
       <c r="AR7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AS7">
-        <v>1340.2</v>
+        <v>1660.85</v>
       </c>
       <c r="AT7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="AU7">
-        <v>2631.45</v>
+        <v>4743.47</v>
       </c>
       <c r="AV7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="AW7">
-        <v>9371.8799999999992</v>
+        <v>11778.9</v>
       </c>
       <c r="AX7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="AY7">
-        <v>751.91800000000001</v>
+        <v>873.99400000000003</v>
       </c>
       <c r="AZ7" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="BA7">
-        <v>149290</v>
+        <v>357423</v>
       </c>
       <c r="BB7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="BC7">
-        <v>4364.37</v>
+        <v>5671.17</v>
       </c>
       <c r="BD7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="BE7">
-        <v>50042.7</v>
+        <v>70232.600000000006</v>
       </c>
       <c r="BF7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9196.7999999999993</v>
+        <v>8997</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C9">
-        <v>170135</v>
+        <v>141504</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E9">
-        <v>8570.57</v>
+        <v>8166.9</v>
       </c>
       <c r="F9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G9">
-        <v>9392.58</v>
+        <v>7450.98</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I9">
-        <v>26107.200000000001</v>
+        <v>19626.900000000001</v>
       </c>
       <c r="J9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K9">
-        <v>900.46100000000001</v>
+        <v>810.07</v>
       </c>
       <c r="L9" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M9">
-        <v>29557.5</v>
+        <v>27133</v>
       </c>
       <c r="N9" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="O9">
-        <v>45719.4</v>
+        <v>32139.5</v>
       </c>
       <c r="P9" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="Q9">
-        <v>66670.5</v>
+        <v>36648.199999999997</v>
       </c>
       <c r="R9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="S9">
-        <v>31799.4</v>
+        <v>26781.3</v>
       </c>
       <c r="T9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="U9">
-        <v>58402.1</v>
+        <v>35342.300000000003</v>
       </c>
       <c r="V9" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="W9">
-        <v>61023.1</v>
+        <v>35581.1</v>
       </c>
       <c r="X9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="Y9">
-        <v>33507.599999999999</v>
+        <v>27886.799999999999</v>
       </c>
       <c r="Z9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="AA9">
-        <v>32925.9</v>
+        <v>29201.5</v>
       </c>
       <c r="AB9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="AC9">
-        <v>32892</v>
+        <v>30572.1</v>
       </c>
       <c r="AD9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AE9">
-        <v>21754.3</v>
+        <v>17000.400000000001</v>
       </c>
       <c r="AF9" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AG9">
-        <v>156732</v>
+        <v>147762</v>
       </c>
       <c r="AH9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AI9">
-        <v>108680</v>
+        <v>51452.3</v>
       </c>
       <c r="AJ9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AK9">
-        <v>132347</v>
+        <v>67828.5</v>
       </c>
       <c r="AL9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AM9">
-        <v>174101</v>
+        <v>126479</v>
       </c>
       <c r="AN9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AO9">
-        <v>189207</v>
+        <v>63459</v>
       </c>
       <c r="AP9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="AQ9">
-        <v>230445</v>
+        <v>87144.2</v>
       </c>
       <c r="AR9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="AS9">
-        <v>1562.43</v>
+        <v>1533.56</v>
       </c>
       <c r="AT9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="AU9">
-        <v>4166.6099999999997</v>
+        <v>2819.26</v>
       </c>
       <c r="AV9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="AW9">
-        <v>11014.9</v>
+        <v>9971.77</v>
       </c>
       <c r="AX9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="AY9">
-        <v>1020.18</v>
+        <v>832.28800000000001</v>
       </c>
       <c r="AZ9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="BA9">
-        <v>307810</v>
+        <v>151797</v>
       </c>
       <c r="BB9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="BC9">
-        <v>6158.34</v>
+        <v>4865.97</v>
       </c>
       <c r="BD9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="BE9">
-        <v>73013.2</v>
+        <v>55031.7</v>
       </c>
       <c r="BF9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9162.8700000000008</v>
+        <v>7663.59</v>
       </c>
       <c r="B11" t="s">
         <v>160</v>
       </c>
       <c r="C11">
-        <v>141607</v>
+        <v>401342</v>
       </c>
       <c r="D11" t="s">
         <v>161</v>
       </c>
       <c r="E11">
-        <v>7497.62</v>
+        <v>6477.58</v>
       </c>
       <c r="F11" t="s">
         <v>162</v>
       </c>
       <c r="G11">
-        <v>8222.15</v>
+        <v>6774.05</v>
       </c>
       <c r="H11" t="s">
         <v>163</v>
       </c>
       <c r="I11">
-        <v>18363.599999999999</v>
+        <v>17203.8</v>
       </c>
       <c r="J11" t="s">
         <v>164</v>
       </c>
       <c r="K11">
-        <v>810.07</v>
+        <v>2073.54</v>
       </c>
       <c r="L11" t="s">
         <v>165</v>
       </c>
       <c r="M11">
-        <v>27018.3</v>
+        <v>190660</v>
       </c>
       <c r="N11" t="s">
         <v>166</v>
       </c>
       <c r="O11">
-        <v>33177.4</v>
+        <v>288430</v>
       </c>
       <c r="P11" t="s">
         <v>167</v>
       </c>
       <c r="Q11">
-        <v>36051.599999999999</v>
+        <v>369916</v>
       </c>
       <c r="R11" t="s">
         <v>168</v>
       </c>
       <c r="S11">
-        <v>27490.9</v>
+        <v>156621</v>
       </c>
       <c r="T11" t="s">
         <v>169</v>
       </c>
       <c r="U11">
-        <v>36466.1</v>
+        <v>271092</v>
       </c>
       <c r="V11" t="s">
         <v>170</v>
       </c>
       <c r="W11">
-        <v>38311.4</v>
+        <v>325294</v>
       </c>
       <c r="X11" t="s">
         <v>171</v>
       </c>
       <c r="Y11">
-        <v>25138.799999999999</v>
+        <v>180539</v>
       </c>
       <c r="Z11" t="s">
         <v>172</v>
       </c>
       <c r="AA11">
-        <v>27874.2</v>
+        <v>169871</v>
       </c>
       <c r="AB11" t="s">
         <v>173</v>
       </c>
       <c r="AC11">
-        <v>28374.3</v>
+        <v>183291</v>
       </c>
       <c r="AD11" t="s">
         <v>174</v>
       </c>
       <c r="AE11">
-        <v>19425.8</v>
+        <v>36316.400000000001</v>
       </c>
       <c r="AF11" t="s">
         <v>175</v>
       </c>
       <c r="AG11">
-        <v>86247.3</v>
+        <v>201351</v>
       </c>
       <c r="AH11" t="s">
         <v>176</v>
       </c>
       <c r="AI11">
-        <v>53182.8</v>
+        <v>64415.1</v>
       </c>
       <c r="AJ11" t="s">
         <v>177</v>
       </c>
       <c r="AK11">
-        <v>70596.899999999994</v>
+        <v>111067</v>
       </c>
       <c r="AL11" t="s">
         <v>178</v>
       </c>
       <c r="AM11">
-        <v>124714</v>
+        <v>295552</v>
       </c>
       <c r="AN11" t="s">
         <v>179</v>
       </c>
       <c r="AO11">
-        <v>64525.5</v>
+        <v>108013</v>
       </c>
       <c r="AP11" t="s">
         <v>180</v>
       </c>
       <c r="AQ11">
-        <v>50642.3</v>
+        <v>182670</v>
       </c>
       <c r="AR11" t="s">
         <v>181</v>
       </c>
       <c r="AS11">
-        <v>1475.8</v>
+        <v>2374.52</v>
       </c>
       <c r="AT11" t="s">
         <v>182</v>
       </c>
       <c r="AU11">
-        <v>2823.35</v>
+        <v>4268.93</v>
       </c>
       <c r="AV11" t="s">
         <v>183</v>
       </c>
       <c r="AW11">
-        <v>10039.6</v>
+        <v>8435.66</v>
       </c>
       <c r="AX11" t="s">
         <v>184</v>
       </c>
       <c r="AY11">
-        <v>852.27099999999996</v>
+        <v>3458.2</v>
       </c>
       <c r="AZ11" t="s">
         <v>185</v>
       </c>
       <c r="BA11">
-        <v>151669</v>
+        <v>305007</v>
       </c>
       <c r="BB11" t="s">
         <v>186</v>
       </c>
       <c r="BC11">
-        <v>4946.16</v>
+        <v>4139.3999999999996</v>
       </c>
       <c r="BD11" t="s">
         <v>187</v>
       </c>
       <c r="BE11">
-        <v>50656.3</v>
+        <v>43254.9</v>
       </c>
       <c r="BF11" t="s">
         <v>188</v>

</xml_diff>